<commit_message>
Linear Regression model code
</commit_message>
<xml_diff>
--- a/data/raw/Enrolled_Students.xlsx
+++ b/data/raw/Enrolled_Students.xlsx
@@ -377,171 +377,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2007</v>
       </c>
       <c r="B2">
-        <v>2007</v>
-      </c>
-      <c r="C2">
         <v>1985546</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>1</v>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2008</v>
       </c>
       <c r="B3">
-        <v>2008</v>
-      </c>
-      <c r="C3">
         <v>2161485</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>2</v>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2009</v>
       </c>
       <c r="B4">
-        <v>2009</v>
-      </c>
-      <c r="C4">
         <v>2058218</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>3</v>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2010</v>
       </c>
       <c r="B5">
-        <v>2010</v>
-      </c>
-      <c r="C5">
         <v>2151856</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>4</v>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2011</v>
       </c>
       <c r="B6">
-        <v>2011</v>
-      </c>
-      <c r="C6">
         <v>2100842</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>5</v>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2012</v>
       </c>
       <c r="B7">
-        <v>2012</v>
-      </c>
-      <c r="C7">
         <v>2120753</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>6</v>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2013</v>
       </c>
       <c r="B8">
-        <v>2013</v>
-      </c>
-      <c r="C8">
         <v>1961891</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1">
-        <v>7</v>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>2014</v>
       </c>
       <c r="B9">
-        <v>2014</v>
-      </c>
-      <c r="C9">
         <v>1960782</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1">
-        <v>8</v>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>2015</v>
       </c>
       <c r="B10">
-        <v>2015</v>
-      </c>
-      <c r="C10">
         <v>2052675</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1">
-        <v>9</v>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2016</v>
       </c>
       <c r="B11">
-        <v>2016</v>
-      </c>
-      <c r="C11">
         <v>2188376</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1">
-        <v>10</v>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>2017</v>
       </c>
       <c r="B12">
-        <v>2017</v>
-      </c>
-      <c r="C12">
         <v>1914747</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1">
-        <v>11</v>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>2018</v>
       </c>
       <c r="B13">
-        <v>2018</v>
-      </c>
-      <c r="C13">
         <v>2220228</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1">
-        <v>12</v>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>2019</v>
       </c>
       <c r="B14">
-        <v>2019</v>
-      </c>
-      <c r="C14">
         <v>2077594</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1">
-        <v>13</v>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>2020</v>
       </c>
       <c r="B15">
-        <v>2020</v>
-      </c>
-      <c r="C15">
         <v>2078283</v>
       </c>
     </row>

</xml_diff>